<commit_message>
The up-to-date time sheet of Noah Greupner.
</commit_message>
<xml_diff>
--- a/Project_management/ip_sdi_time_sheet_s1095729__1_.xlsx
+++ b/Project_management/ip_sdi_time_sheet_s1095729__1_.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27217"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27226"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_3219\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="168" documentId="8_{FB00358B-D802-4A23-B5B0-D35ABEF17C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4A193DB-C18A-4F65-8C62-A99E95F73C67}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="8_{FB00358B-D802-4A23-B5B0-D35ABEF17C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EF2BC29-6523-4BD8-ADD6-3B918F7179D7}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" tabRatio="893" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" tabRatio="893" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="October" sheetId="7" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="74">
   <si>
     <t>Monthly timesheet for MSc Geoinformatics ip:sdi - 23W856162</t>
   </si>
@@ -277,6 +277,15 @@
   </si>
   <si>
     <t>WP0: update GitLab and project management documents</t>
+  </si>
+  <si>
+    <t>WP4: dealing with ArcGIS Insights</t>
+  </si>
+  <si>
+    <t>WP4: dashboard layout</t>
+  </si>
+  <si>
+    <t>WP0 and WP4</t>
   </si>
 </sst>
 </file>
@@ -760,7 +769,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -820,6 +829,102 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="5" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -838,6 +943,36 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="167" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -847,131 +982,27 @@
     <xf numFmtId="167" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1353,7 +1384,7 @@
   </sheetPr>
   <dimension ref="A1:AW50"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A29" zoomScale="120" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A8" zoomScale="120" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
       <selection activeCell="A11" sqref="A11:C11"/>
     </sheetView>
   </sheetViews>
@@ -1374,17 +1405,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:49" s="6" customFormat="1" ht="18.75" thickBot="1">
-      <c r="A1" s="81" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -1427,120 +1458,120 @@
       <c r="AW1" s="1"/>
     </row>
     <row r="2" spans="1:49" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A2" s="82"/>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
     </row>
     <row r="3" spans="1:49" s="7" customFormat="1" ht="13.7" customHeight="1">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="83"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="14"/>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
     </row>
     <row r="4" spans="1:49" s="1" customFormat="1" ht="9" customHeight="1">
-      <c r="A4" s="84"/>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
     </row>
     <row r="5" spans="1:49" s="1" customFormat="1" ht="13.9" customHeight="1">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="75" t="s">
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="76"/>
-      <c r="H5" s="77"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="45"/>
       <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:49" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A6" s="78"/>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
     </row>
     <row r="7" spans="1:49" s="1" customFormat="1" ht="13.9" customHeight="1">
-      <c r="A7" s="79" t="s">
+      <c r="A7" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="80" t="s">
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="80"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
       <c r="I7" s="15"/>
     </row>
     <row r="8" spans="1:49" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A8" s="85"/>
-      <c r="B8" s="85"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="85"/>
-      <c r="H8" s="85"/>
-      <c r="I8" s="85"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
     </row>
     <row r="9" spans="1:49" s="1" customFormat="1" ht="13.9" customHeight="1">
-      <c r="A9" s="79" t="s">
+      <c r="A9" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="75" t="s">
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="76"/>
-      <c r="F9" s="76"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="77"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="45"/>
       <c r="I9" s="15"/>
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:49" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A10" s="72"/>
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="72"/>
-      <c r="G10" s="72"/>
-      <c r="H10" s="72"/>
-      <c r="I10" s="72"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
     </row>
     <row r="11" spans="1:49" s="1" customFormat="1" ht="12.75">
       <c r="A11" s="34" t="s">
@@ -1569,51 +1600,51 @@
       <c r="I12" s="16"/>
     </row>
     <row r="13" spans="1:49" s="2" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="60" t="s">
+      <c r="B13" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="62"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="54"/>
     </row>
     <row r="14" spans="1:49" s="2" customFormat="1" ht="13.9" customHeight="1">
-      <c r="A14" s="58"/>
-      <c r="B14" s="63" t="s">
+      <c r="A14" s="50"/>
+      <c r="B14" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="86"/>
-      <c r="D14" s="64" t="s">
+      <c r="C14" s="96"/>
+      <c r="D14" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="66" t="s">
+      <c r="E14" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="67"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="67"/>
-      <c r="I14" s="68"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="60"/>
     </row>
     <row r="15" spans="1:49" ht="13.35" customHeight="1">
-      <c r="A15" s="59"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="65"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="70"/>
-      <c r="H15" s="70"/>
-      <c r="I15" s="71"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="63"/>
     </row>
     <row r="16" spans="1:49" s="32" customFormat="1" ht="12.75">
       <c r="A16" s="29" t="s">
@@ -1625,11 +1656,11 @@
         <f>C16-B16</f>
         <v>0</v>
       </c>
-      <c r="E16" s="56"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="40"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="71"/>
+      <c r="G16" s="71"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="72"/>
     </row>
     <row r="17" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A17" s="29" t="s">
@@ -1641,11 +1672,11 @@
         <f t="shared" ref="D17:D46" si="0">C17-B17</f>
         <v>0</v>
       </c>
-      <c r="E17" s="38"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="40"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="71"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="72"/>
     </row>
     <row r="18" spans="1:9" s="28" customFormat="1" ht="12.75">
       <c r="A18" s="25" t="s">
@@ -1657,13 +1688,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E18" s="53" t="s">
+      <c r="E18" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="54"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="55"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="66"/>
     </row>
     <row r="19" spans="1:9" s="28" customFormat="1" ht="12.75">
       <c r="A19" s="25" t="s">
@@ -1675,11 +1706,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E19" s="35"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="37"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="68"/>
+      <c r="G19" s="68"/>
+      <c r="H19" s="68"/>
+      <c r="I19" s="69"/>
     </row>
     <row r="20" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A20" s="29" t="s">
@@ -1695,13 +1726,13 @@
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="E20" s="38" t="s">
+      <c r="E20" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="40"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="72"/>
     </row>
     <row r="21" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A21" s="29" t="s">
@@ -1717,13 +1748,13 @@
         <f t="shared" si="0"/>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="E21" s="50" t="s">
+      <c r="E21" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="51"/>
-      <c r="I21" s="52"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="75"/>
+      <c r="H21" s="75"/>
+      <c r="I21" s="76"/>
     </row>
     <row r="22" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A22" s="29" t="s">
@@ -1735,11 +1766,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E22" s="38"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="40"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="72"/>
     </row>
     <row r="23" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A23" s="29" t="s">
@@ -1751,11 +1782,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E23" s="38"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="40"/>
+      <c r="E23" s="70"/>
+      <c r="F23" s="71"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="72"/>
     </row>
     <row r="24" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A24" s="29" t="s">
@@ -1767,11 +1798,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E24" s="38"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="40"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="72"/>
     </row>
     <row r="25" spans="1:9" s="28" customFormat="1" ht="12.75">
       <c r="A25" s="25" t="s">
@@ -1783,11 +1814,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E25" s="35"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="37"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="69"/>
     </row>
     <row r="26" spans="1:9" s="28" customFormat="1" ht="12.75">
       <c r="A26" s="25" t="s">
@@ -1799,11 +1830,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E26" s="35"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="37"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="69"/>
     </row>
     <row r="27" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A27" s="29" t="s">
@@ -1819,13 +1850,13 @@
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E27" s="38" t="s">
+      <c r="E27" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="40"/>
+      <c r="F27" s="71"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="71"/>
+      <c r="I27" s="72"/>
     </row>
     <row r="28" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A28" s="29" t="s">
@@ -1837,11 +1868,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E28" s="38"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="40"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="72"/>
     </row>
     <row r="29" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A29" s="29" t="s">
@@ -1853,11 +1884,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E29" s="38"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="40"/>
+      <c r="E29" s="70"/>
+      <c r="F29" s="71"/>
+      <c r="G29" s="71"/>
+      <c r="H29" s="71"/>
+      <c r="I29" s="72"/>
     </row>
     <row r="30" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A30" s="29" t="s">
@@ -1873,13 +1904,13 @@
         <f t="shared" si="0"/>
         <v>8.3333333333333315E-2</v>
       </c>
-      <c r="E30" s="44" t="s">
+      <c r="E30" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="46"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="78"/>
+      <c r="H30" s="78"/>
+      <c r="I30" s="79"/>
     </row>
     <row r="31" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A31" s="29" t="s">
@@ -1895,13 +1926,13 @@
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="E31" s="47" t="s">
+      <c r="E31" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="48"/>
-      <c r="I31" s="49"/>
+      <c r="F31" s="81"/>
+      <c r="G31" s="81"/>
+      <c r="H31" s="81"/>
+      <c r="I31" s="82"/>
     </row>
     <row r="32" spans="1:9" s="28" customFormat="1" ht="12.75">
       <c r="A32" s="25" t="s">
@@ -1913,11 +1944,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E32" s="35"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="37"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="68"/>
+      <c r="G32" s="68"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="69"/>
     </row>
     <row r="33" spans="1:13" s="28" customFormat="1" ht="12.75">
       <c r="A33" s="25" t="s">
@@ -1929,11 +1960,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E33" s="35"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="37"/>
+      <c r="E33" s="67"/>
+      <c r="F33" s="68"/>
+      <c r="G33" s="68"/>
+      <c r="H33" s="68"/>
+      <c r="I33" s="69"/>
     </row>
     <row r="34" spans="1:13" s="32" customFormat="1" ht="12.75">
       <c r="A34" s="29" t="s">
@@ -1945,11 +1976,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E34" s="38"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="39"/>
-      <c r="I34" s="40"/>
+      <c r="E34" s="70"/>
+      <c r="F34" s="71"/>
+      <c r="G34" s="71"/>
+      <c r="H34" s="71"/>
+      <c r="I34" s="72"/>
     </row>
     <row r="35" spans="1:13" s="32" customFormat="1" ht="12.75">
       <c r="A35" s="29" t="s">
@@ -1961,11 +1992,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E35" s="38"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="40"/>
+      <c r="E35" s="70"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="71"/>
+      <c r="H35" s="71"/>
+      <c r="I35" s="72"/>
     </row>
     <row r="36" spans="1:13" s="32" customFormat="1" ht="12.75">
       <c r="A36" s="29" t="s">
@@ -1981,13 +2012,13 @@
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E36" s="38" t="s">
+      <c r="E36" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="F36" s="39"/>
-      <c r="G36" s="39"/>
-      <c r="H36" s="39"/>
-      <c r="I36" s="40"/>
+      <c r="F36" s="71"/>
+      <c r="G36" s="71"/>
+      <c r="H36" s="71"/>
+      <c r="I36" s="72"/>
     </row>
     <row r="37" spans="1:13" s="32" customFormat="1" ht="12.75">
       <c r="A37" s="29" t="s">
@@ -1999,11 +2030,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E37" s="38"/>
-      <c r="F37" s="39"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="39"/>
-      <c r="I37" s="40"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="71"/>
+      <c r="G37" s="71"/>
+      <c r="H37" s="71"/>
+      <c r="I37" s="72"/>
     </row>
     <row r="38" spans="1:13" s="32" customFormat="1" ht="12.75">
       <c r="A38" s="29" t="s">
@@ -2015,11 +2046,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E38" s="38"/>
-      <c r="F38" s="39"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="39"/>
-      <c r="I38" s="40"/>
+      <c r="E38" s="70"/>
+      <c r="F38" s="71"/>
+      <c r="G38" s="71"/>
+      <c r="H38" s="71"/>
+      <c r="I38" s="72"/>
     </row>
     <row r="39" spans="1:13" s="28" customFormat="1" ht="12.75">
       <c r="A39" s="25" t="s">
@@ -2031,11 +2062,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E39" s="35"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="37"/>
+      <c r="E39" s="67"/>
+      <c r="F39" s="68"/>
+      <c r="G39" s="68"/>
+      <c r="H39" s="68"/>
+      <c r="I39" s="69"/>
     </row>
     <row r="40" spans="1:13" s="28" customFormat="1" ht="12.75">
       <c r="A40" s="25" t="s">
@@ -2047,11 +2078,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E40" s="35"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="37"/>
+      <c r="E40" s="67"/>
+      <c r="F40" s="68"/>
+      <c r="G40" s="68"/>
+      <c r="H40" s="68"/>
+      <c r="I40" s="69"/>
     </row>
     <row r="41" spans="1:13" s="32" customFormat="1" ht="12.75">
       <c r="A41" s="29" t="s">
@@ -2063,11 +2094,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E41" s="38"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="39"/>
-      <c r="H41" s="39"/>
-      <c r="I41" s="40"/>
+      <c r="E41" s="70"/>
+      <c r="F41" s="71"/>
+      <c r="G41" s="71"/>
+      <c r="H41" s="71"/>
+      <c r="I41" s="72"/>
     </row>
     <row r="42" spans="1:13" s="32" customFormat="1" ht="12.75">
       <c r="A42" s="29" t="s">
@@ -2079,11 +2110,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E42" s="38"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="39"/>
-      <c r="I42" s="40"/>
+      <c r="E42" s="70"/>
+      <c r="F42" s="71"/>
+      <c r="G42" s="71"/>
+      <c r="H42" s="71"/>
+      <c r="I42" s="72"/>
     </row>
     <row r="43" spans="1:13" s="32" customFormat="1" ht="12.75">
       <c r="A43" s="29" t="s">
@@ -2095,11 +2126,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E43" s="38"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="39"/>
-      <c r="H43" s="39"/>
-      <c r="I43" s="40"/>
+      <c r="E43" s="70"/>
+      <c r="F43" s="71"/>
+      <c r="G43" s="71"/>
+      <c r="H43" s="71"/>
+      <c r="I43" s="72"/>
     </row>
     <row r="44" spans="1:13" s="32" customFormat="1" ht="12.75">
       <c r="A44" s="29" t="s">
@@ -2111,11 +2142,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E44" s="38"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="40"/>
+      <c r="E44" s="70"/>
+      <c r="F44" s="71"/>
+      <c r="G44" s="71"/>
+      <c r="H44" s="71"/>
+      <c r="I44" s="72"/>
     </row>
     <row r="45" spans="1:13" s="32" customFormat="1" ht="12.75">
       <c r="A45" s="29" t="s">
@@ -2131,13 +2162,13 @@
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E45" s="38" t="s">
+      <c r="E45" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="F45" s="39"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="39"/>
-      <c r="I45" s="40"/>
+      <c r="F45" s="71"/>
+      <c r="G45" s="71"/>
+      <c r="H45" s="71"/>
+      <c r="I45" s="72"/>
     </row>
     <row r="46" spans="1:13" s="28" customFormat="1" ht="12.75">
       <c r="A46" s="25" t="s">
@@ -2149,25 +2180,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E46" s="35"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="36"/>
-      <c r="I46" s="37"/>
+      <c r="E46" s="67"/>
+      <c r="F46" s="68"/>
+      <c r="G46" s="68"/>
+      <c r="H46" s="68"/>
+      <c r="I46" s="69"/>
     </row>
     <row r="47" spans="1:13" s="24" customFormat="1" ht="15">
-      <c r="A47" s="41"/>
-      <c r="B47" s="42"/>
-      <c r="C47" s="42"/>
+      <c r="A47" s="83"/>
+      <c r="B47" s="84"/>
+      <c r="C47" s="84"/>
       <c r="D47" s="23">
         <f>SUM(D16:D46)</f>
         <v>0.5</v>
       </c>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="43"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="87"/>
+      <c r="E47" s="85"/>
+      <c r="F47" s="85"/>
+      <c r="G47" s="85"/>
+      <c r="H47" s="85"/>
+      <c r="I47" s="97"/>
     </row>
     <row r="48" spans="1:13" ht="7.5" customHeight="1">
       <c r="A48" s="18"/>
@@ -2198,35 +2229,19 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:I15"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E39:I39"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="E41:I41"/>
+    <mergeCell ref="E36:I36"/>
+    <mergeCell ref="E37:I37"/>
+    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="E45:I45"/>
+    <mergeCell ref="E46:I46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="E47:I47"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="E44:I44"/>
     <mergeCell ref="E35:I35"/>
     <mergeCell ref="E30:I30"/>
     <mergeCell ref="E31:I31"/>
@@ -2236,19 +2251,35 @@
     <mergeCell ref="E29:I29"/>
     <mergeCell ref="E33:I33"/>
     <mergeCell ref="E34:I34"/>
-    <mergeCell ref="E45:I45"/>
-    <mergeCell ref="E46:I46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="E47:I47"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="E39:I39"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="E41:I41"/>
-    <mergeCell ref="E36:I36"/>
-    <mergeCell ref="E37:I37"/>
-    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:I15"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A8:I8"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.44" right="0.03" top="0.02" bottom="0.03" header="0.19685039370078741" footer="0.19685039370078741"/>
@@ -2264,8 +2295,8 @@
   </sheetPr>
   <dimension ref="A1:AR47"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="120" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38:I38"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A5" zoomScale="120" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40:I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -2284,18 +2315,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" s="6" customFormat="1" ht="18.75" thickBot="1">
-      <c r="A1" s="81" t="str">
+      <c r="A1" s="35" t="str">
         <f>October!A1</f>
         <v>Monthly timesheet for MSc Geoinformatics ip:sdi - 23W856162</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -2333,126 +2364,126 @@
       <c r="AR1" s="1"/>
     </row>
     <row r="2" spans="1:44" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A2" s="82"/>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
     </row>
     <row r="3" spans="1:44" s="7" customFormat="1" ht="13.7" customHeight="1">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="83"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="14"/>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
     </row>
     <row r="4" spans="1:44" s="1" customFormat="1" ht="9" customHeight="1">
-      <c r="A4" s="84"/>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
     </row>
     <row r="5" spans="1:44" s="1" customFormat="1" ht="13.9" customHeight="1">
-      <c r="A5" s="73" t="str">
+      <c r="A5" s="41" t="str">
         <f>October!A5</f>
         <v>Firstname Lastname</v>
       </c>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="75" t="str">
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="43" t="str">
         <f>October!D5</f>
         <v>Noah Greupner</v>
       </c>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="76"/>
-      <c r="H5" s="77"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="45"/>
       <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:44" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A6" s="78"/>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
     </row>
     <row r="7" spans="1:44" s="1" customFormat="1" ht="13.9" customHeight="1">
-      <c r="A7" s="79" t="str">
+      <c r="A7" s="47" t="str">
         <f>October!A7</f>
         <v>Project Acronym</v>
       </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="80" t="str">
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="48" t="str">
         <f>October!D7</f>
         <v>SudMig</v>
       </c>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="80"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
       <c r="I7" s="15"/>
     </row>
     <row r="8" spans="1:44" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A8" s="85"/>
-      <c r="B8" s="85"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="85"/>
-      <c r="H8" s="85"/>
-      <c r="I8" s="85"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
     </row>
     <row r="9" spans="1:44" s="1" customFormat="1" ht="13.9" customHeight="1">
-      <c r="A9" s="79" t="str">
+      <c r="A9" s="47" t="str">
         <f>October!A9</f>
         <v>Project Title</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="75" t="str">
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="43" t="str">
         <f>October!D9</f>
         <v>Sudan: monitoring migrant movements related to the 2023 conflict</v>
       </c>
-      <c r="E9" s="76"/>
-      <c r="F9" s="76"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="77"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="45"/>
       <c r="I9" s="15"/>
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:44" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A10" s="72"/>
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="72"/>
-      <c r="G10" s="72"/>
-      <c r="H10" s="72"/>
-      <c r="I10" s="72"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
     </row>
     <row r="11" spans="1:44" s="1" customFormat="1" ht="12.75">
       <c r="A11" s="34" t="s">
@@ -2482,51 +2513,51 @@
       <c r="I12" s="16"/>
     </row>
     <row r="13" spans="1:44" s="2" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="60" t="s">
+      <c r="B13" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="62"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="54"/>
     </row>
     <row r="14" spans="1:44" s="2" customFormat="1" ht="13.9" customHeight="1">
-      <c r="A14" s="58"/>
-      <c r="B14" s="63" t="s">
+      <c r="A14" s="50"/>
+      <c r="B14" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="86"/>
-      <c r="D14" s="64" t="s">
+      <c r="C14" s="96"/>
+      <c r="D14" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="66" t="s">
+      <c r="E14" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="67"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="67"/>
-      <c r="I14" s="68"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="60"/>
     </row>
     <row r="15" spans="1:44" ht="13.35" customHeight="1">
-      <c r="A15" s="59"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="65"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="70"/>
-      <c r="H15" s="70"/>
-      <c r="I15" s="71"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="63"/>
     </row>
     <row r="16" spans="1:44" s="28" customFormat="1" ht="12.75">
       <c r="A16" s="25" t="s">
@@ -2538,11 +2569,11 @@
         <f>C16-B16</f>
         <v>0</v>
       </c>
-      <c r="E16" s="35"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="37"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="69"/>
     </row>
     <row r="17" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A17" s="29" t="s">
@@ -2554,11 +2585,11 @@
         <f t="shared" ref="D17:D45" si="0">C17-B17</f>
         <v>0</v>
       </c>
-      <c r="E17" s="38"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="40"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="71"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="72"/>
     </row>
     <row r="18" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A18" s="29" t="s">
@@ -2574,13 +2605,13 @@
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E18" s="38" t="s">
+      <c r="E18" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="40"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="72"/>
     </row>
     <row r="19" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A19" s="29" t="s">
@@ -2592,11 +2623,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E19" s="38"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="40"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="72"/>
     </row>
     <row r="20" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A20" s="29" t="s">
@@ -2608,11 +2639,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="40"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="72"/>
     </row>
     <row r="21" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A21" s="29" t="s">
@@ -2628,13 +2659,13 @@
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E21" s="38" t="s">
+      <c r="E21" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="40"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="72"/>
     </row>
     <row r="22" spans="1:9" s="28" customFormat="1" ht="12.75">
       <c r="A22" s="25" t="s">
@@ -2650,13 +2681,13 @@
         <f t="shared" si="0"/>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="E22" s="35" t="s">
+      <c r="E22" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="37"/>
+      <c r="F22" s="68"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="68"/>
+      <c r="I22" s="69"/>
     </row>
     <row r="23" spans="1:9" s="28" customFormat="1" ht="12.75">
       <c r="A23" s="25" t="s">
@@ -2668,11 +2699,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E23" s="35"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="37"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="69"/>
     </row>
     <row r="24" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A24" s="29" t="s">
@@ -2688,13 +2719,13 @@
         <f t="shared" si="0"/>
         <v>2.083333333333337E-2</v>
       </c>
-      <c r="E24" s="38" t="s">
+      <c r="E24" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="40"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="72"/>
     </row>
     <row r="25" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A25" s="29" t="s">
@@ -2706,11 +2737,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E25" s="38"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="40"/>
+      <c r="E25" s="70"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="72"/>
     </row>
     <row r="26" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A26" s="29" t="s">
@@ -2726,13 +2757,13 @@
         <f t="shared" si="0"/>
         <v>4.1666666666666741E-2</v>
       </c>
-      <c r="E26" s="38" t="s">
+      <c r="E26" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="40"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="72"/>
     </row>
     <row r="27" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A27" s="29" t="s">
@@ -2744,11 +2775,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27" s="38"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="40"/>
+      <c r="E27" s="70"/>
+      <c r="F27" s="71"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="71"/>
+      <c r="I27" s="72"/>
     </row>
     <row r="28" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A28" s="29" t="s">
@@ -2760,11 +2791,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E28" s="38"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="40"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="72"/>
     </row>
     <row r="29" spans="1:9" s="28" customFormat="1" ht="12.75">
       <c r="A29" s="25" t="s">
@@ -2776,11 +2807,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E29" s="35"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="37"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="68"/>
+      <c r="G29" s="68"/>
+      <c r="H29" s="68"/>
+      <c r="I29" s="69"/>
     </row>
     <row r="30" spans="1:9" s="28" customFormat="1" ht="12.75">
       <c r="A30" s="25" t="s">
@@ -2796,13 +2827,13 @@
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E30" s="35" t="s">
+      <c r="E30" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="37"/>
+      <c r="F30" s="68"/>
+      <c r="G30" s="68"/>
+      <c r="H30" s="68"/>
+      <c r="I30" s="69"/>
     </row>
     <row r="31" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A31" s="29" t="s">
@@ -2814,11 +2845,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E31" s="38"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="40"/>
+      <c r="E31" s="70"/>
+      <c r="F31" s="71"/>
+      <c r="G31" s="71"/>
+      <c r="H31" s="71"/>
+      <c r="I31" s="72"/>
     </row>
     <row r="32" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A32" s="29" t="s">
@@ -2834,13 +2865,13 @@
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="E32" s="38" t="s">
+      <c r="E32" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="40"/>
+      <c r="F32" s="71"/>
+      <c r="G32" s="71"/>
+      <c r="H32" s="71"/>
+      <c r="I32" s="72"/>
     </row>
     <row r="33" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A33" s="29" t="s">
@@ -2852,11 +2883,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E33" s="38"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="40"/>
+      <c r="E33" s="70"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="71"/>
+      <c r="I33" s="72"/>
     </row>
     <row r="34" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A34" s="29" t="s">
@@ -2868,11 +2899,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E34" s="38"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="39"/>
-      <c r="I34" s="40"/>
+      <c r="E34" s="70"/>
+      <c r="F34" s="71"/>
+      <c r="G34" s="71"/>
+      <c r="H34" s="71"/>
+      <c r="I34" s="72"/>
     </row>
     <row r="35" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A35" s="29" t="s">
@@ -2884,11 +2915,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E35" s="38"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="40"/>
+      <c r="E35" s="70"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="71"/>
+      <c r="H35" s="71"/>
+      <c r="I35" s="72"/>
     </row>
     <row r="36" spans="1:12" s="28" customFormat="1" ht="12.75">
       <c r="A36" s="25" t="s">
@@ -2900,11 +2931,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E36" s="35"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="37"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="68"/>
+      <c r="G36" s="68"/>
+      <c r="H36" s="68"/>
+      <c r="I36" s="69"/>
     </row>
     <row r="37" spans="1:12" s="28" customFormat="1" ht="12.75">
       <c r="A37" s="25" t="s">
@@ -2920,13 +2951,13 @@
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="E37" s="35" t="s">
+      <c r="E37" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="37"/>
+      <c r="F37" s="68"/>
+      <c r="G37" s="68"/>
+      <c r="H37" s="68"/>
+      <c r="I37" s="69"/>
     </row>
     <row r="38" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A38" s="29" t="s">
@@ -2938,11 +2969,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E38" s="38"/>
-      <c r="F38" s="39"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="39"/>
-      <c r="I38" s="40"/>
+      <c r="E38" s="70"/>
+      <c r="F38" s="71"/>
+      <c r="G38" s="71"/>
+      <c r="H38" s="71"/>
+      <c r="I38" s="72"/>
     </row>
     <row r="39" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A39" s="29" t="s">
@@ -2954,11 +2985,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E39" s="38"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="39"/>
-      <c r="I39" s="40"/>
+      <c r="E39" s="70"/>
+      <c r="F39" s="71"/>
+      <c r="G39" s="71"/>
+      <c r="H39" s="71"/>
+      <c r="I39" s="72"/>
     </row>
     <row r="40" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A40" s="29" t="s">
@@ -2974,13 +3005,13 @@
         <f t="shared" si="0"/>
         <v>4.1666666666666685E-2</v>
       </c>
-      <c r="E40" s="38" t="s">
+      <c r="E40" s="70" t="s">
         <v>63</v>
       </c>
-      <c r="F40" s="39"/>
-      <c r="G40" s="39"/>
-      <c r="H40" s="39"/>
-      <c r="I40" s="40"/>
+      <c r="F40" s="71"/>
+      <c r="G40" s="71"/>
+      <c r="H40" s="71"/>
+      <c r="I40" s="72"/>
     </row>
     <row r="41" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A41" s="29" t="s">
@@ -2992,11 +3023,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E41" s="38"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="39"/>
-      <c r="H41" s="39"/>
-      <c r="I41" s="40"/>
+      <c r="E41" s="70"/>
+      <c r="F41" s="71"/>
+      <c r="G41" s="71"/>
+      <c r="H41" s="71"/>
+      <c r="I41" s="72"/>
     </row>
     <row r="42" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A42" s="29" t="s">
@@ -3012,13 +3043,13 @@
         <f t="shared" si="0"/>
         <v>2.0833333333333259E-2</v>
       </c>
-      <c r="E42" s="38" t="s">
+      <c r="E42" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="39"/>
-      <c r="I42" s="40"/>
+      <c r="F42" s="71"/>
+      <c r="G42" s="71"/>
+      <c r="H42" s="71"/>
+      <c r="I42" s="72"/>
     </row>
     <row r="43" spans="1:12" s="28" customFormat="1" ht="12.75">
       <c r="A43" s="25" t="s">
@@ -3034,13 +3065,13 @@
         <f t="shared" si="0"/>
         <v>8.3333333333333259E-2</v>
       </c>
-      <c r="E43" s="35" t="s">
+      <c r="E43" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="37"/>
+      <c r="F43" s="68"/>
+      <c r="G43" s="68"/>
+      <c r="H43" s="68"/>
+      <c r="I43" s="69"/>
     </row>
     <row r="44" spans="1:12" s="28" customFormat="1" ht="12.75">
       <c r="A44" s="25" t="s">
@@ -3056,13 +3087,13 @@
         <f t="shared" si="0"/>
         <v>8.3333333333333259E-2</v>
       </c>
-      <c r="E44" s="35" t="s">
+      <c r="E44" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="37"/>
+      <c r="F44" s="68"/>
+      <c r="G44" s="68"/>
+      <c r="H44" s="68"/>
+      <c r="I44" s="69"/>
     </row>
     <row r="45" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A45" s="29" t="s">
@@ -3074,25 +3105,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E45" s="38"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="39"/>
-      <c r="I45" s="40"/>
+      <c r="E45" s="70"/>
+      <c r="F45" s="71"/>
+      <c r="G45" s="71"/>
+      <c r="H45" s="71"/>
+      <c r="I45" s="72"/>
     </row>
     <row r="46" spans="1:12" s="24" customFormat="1" ht="15">
-      <c r="A46" s="41"/>
-      <c r="B46" s="42"/>
-      <c r="C46" s="42"/>
+      <c r="A46" s="83"/>
+      <c r="B46" s="84"/>
+      <c r="C46" s="84"/>
       <c r="D46" s="23">
         <f>SUM(D16:D45)</f>
         <v>0.70833333333333326</v>
       </c>
-      <c r="E46" s="43"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="43"/>
-      <c r="H46" s="43"/>
-      <c r="I46" s="87"/>
+      <c r="E46" s="85"/>
+      <c r="F46" s="85"/>
+      <c r="G46" s="85"/>
+      <c r="H46" s="85"/>
+      <c r="I46" s="97"/>
     </row>
     <row r="47" spans="1:12" ht="7.15" customHeight="1">
       <c r="A47" s="18"/>
@@ -3110,6 +3141,40 @@
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="E46:I46"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="E45:I45"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="E41:I41"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="E37:I37"/>
+    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="E39:I39"/>
+    <mergeCell ref="E34:I34"/>
+    <mergeCell ref="E35:I35"/>
+    <mergeCell ref="E36:I36"/>
+    <mergeCell ref="E31:I31"/>
+    <mergeCell ref="E32:I32"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E20:I20"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:H3"/>
@@ -3126,40 +3191,6 @@
     <mergeCell ref="E14:I15"/>
     <mergeCell ref="E16:I16"/>
     <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
-    <mergeCell ref="E30:I30"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E35:I35"/>
-    <mergeCell ref="E36:I36"/>
-    <mergeCell ref="E31:I31"/>
-    <mergeCell ref="E32:I32"/>
-    <mergeCell ref="E33:I33"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="E46:I46"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="E45:I45"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="E41:I41"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="E37:I37"/>
-    <mergeCell ref="E38:I38"/>
-    <mergeCell ref="E39:I39"/>
-    <mergeCell ref="E34:I34"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.44" right="0.03" top="0.02" bottom="0.03" header="0.19685039370078741" footer="0.19685039370078741"/>
@@ -3175,8 +3206,8 @@
   </sheetPr>
   <dimension ref="A1:AM48"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="120" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A24" zoomScale="120" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31:I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -3194,18 +3225,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" s="6" customFormat="1" ht="18.75" thickBot="1">
-      <c r="A1" s="81" t="str">
+      <c r="A1" s="35" t="str">
         <f>October!A1</f>
         <v>Monthly timesheet for MSc Geoinformatics ip:sdi - 23W856162</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -3238,126 +3269,126 @@
       <c r="AM1" s="1"/>
     </row>
     <row r="2" spans="1:39" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A2" s="82"/>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
     </row>
     <row r="3" spans="1:39" s="7" customFormat="1" ht="13.7" customHeight="1">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="83"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="14"/>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
     </row>
     <row r="4" spans="1:39" s="1" customFormat="1" ht="9" customHeight="1">
-      <c r="A4" s="84"/>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
     </row>
     <row r="5" spans="1:39" s="1" customFormat="1" ht="13.9" customHeight="1">
-      <c r="A5" s="73" t="str">
+      <c r="A5" s="41" t="str">
         <f>October!A5</f>
         <v>Firstname Lastname</v>
       </c>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="75" t="str">
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="43" t="str">
         <f>October!D5</f>
         <v>Noah Greupner</v>
       </c>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="76"/>
-      <c r="H5" s="77"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="45"/>
       <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:39" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A6" s="78"/>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
     </row>
     <row r="7" spans="1:39" s="1" customFormat="1" ht="13.9" customHeight="1">
-      <c r="A7" s="79" t="str">
+      <c r="A7" s="47" t="str">
         <f>October!A7</f>
         <v>Project Acronym</v>
       </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="80" t="str">
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="48" t="str">
         <f>October!D7</f>
         <v>SudMig</v>
       </c>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="80"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
       <c r="I7" s="15"/>
     </row>
     <row r="8" spans="1:39" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A8" s="85"/>
-      <c r="B8" s="85"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="85"/>
-      <c r="H8" s="85"/>
-      <c r="I8" s="85"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
     </row>
     <row r="9" spans="1:39" s="1" customFormat="1" ht="13.9" customHeight="1">
-      <c r="A9" s="79" t="str">
+      <c r="A9" s="47" t="str">
         <f>October!A9</f>
         <v>Project Title</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="75" t="str">
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="43" t="str">
         <f>October!D9</f>
         <v>Sudan: monitoring migrant movements related to the 2023 conflict</v>
       </c>
-      <c r="E9" s="76"/>
-      <c r="F9" s="76"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="77"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="45"/>
       <c r="I9" s="15"/>
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:39" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A10" s="72"/>
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="72"/>
-      <c r="G10" s="72"/>
-      <c r="H10" s="72"/>
-      <c r="I10" s="72"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
     </row>
     <row r="11" spans="1:39" s="1" customFormat="1" ht="12.75">
       <c r="A11" s="34" t="s">
@@ -3387,591 +3418,615 @@
       <c r="I12" s="16"/>
     </row>
     <row r="13" spans="1:39" s="2" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="60" t="s">
+      <c r="B13" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="62"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="54"/>
     </row>
     <row r="14" spans="1:39" s="2" customFormat="1" ht="13.9" customHeight="1">
-      <c r="A14" s="58"/>
-      <c r="B14" s="63" t="s">
+      <c r="A14" s="50"/>
+      <c r="B14" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="86"/>
-      <c r="D14" s="64" t="s">
+      <c r="C14" s="96"/>
+      <c r="D14" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="66" t="s">
+      <c r="E14" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="67"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="67"/>
-      <c r="I14" s="68"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="60"/>
     </row>
     <row r="15" spans="1:39" ht="13.35" customHeight="1">
-      <c r="A15" s="59"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="65"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="70"/>
-      <c r="H15" s="70"/>
-      <c r="I15" s="71"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="63"/>
     </row>
     <row r="16" spans="1:39" s="32" customFormat="1" ht="12.75">
       <c r="A16" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="30">
+      <c r="B16" s="86">
         <v>0.75</v>
       </c>
-      <c r="C16" s="31">
+      <c r="C16" s="87">
         <v>0.79166666666666663</v>
       </c>
-      <c r="D16" s="31">
+      <c r="D16" s="87">
         <f>C16-B16</f>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="E16" s="38" t="s">
+      <c r="E16" s="88" t="s">
         <v>66</v>
       </c>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="40"/>
+      <c r="F16" s="89"/>
+      <c r="G16" s="89"/>
+      <c r="H16" s="89"/>
+      <c r="I16" s="90"/>
     </row>
     <row r="17" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A17" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31">
+      <c r="B17" s="86"/>
+      <c r="C17" s="87"/>
+      <c r="D17" s="87">
         <f t="shared" ref="D17:D46" si="0">C17-B17</f>
         <v>0</v>
       </c>
-      <c r="E17" s="38"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="40"/>
+      <c r="E17" s="88"/>
+      <c r="F17" s="89"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="89"/>
+      <c r="I17" s="90"/>
     </row>
     <row r="18" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A18" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E18" s="38"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="40"/>
+      <c r="B18" s="86"/>
+      <c r="C18" s="87"/>
+      <c r="D18" s="87">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="88"/>
+      <c r="F18" s="89"/>
+      <c r="G18" s="89"/>
+      <c r="H18" s="89"/>
+      <c r="I18" s="90"/>
     </row>
     <row r="19" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A19" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="30">
+      <c r="B19" s="86">
         <v>0.45833333333333331</v>
       </c>
-      <c r="C19" s="31">
+      <c r="C19" s="87">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D19" s="31">
+      <c r="D19" s="87">
         <f t="shared" si="0"/>
         <v>0.12500000000000006</v>
       </c>
-      <c r="E19" s="38" t="s">
+      <c r="E19" s="88" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="40"/>
+      <c r="F19" s="89"/>
+      <c r="G19" s="89"/>
+      <c r="H19" s="89"/>
+      <c r="I19" s="90"/>
     </row>
     <row r="20" spans="1:9" s="28" customFormat="1" ht="12.75">
       <c r="A20" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E20" s="35"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="37"/>
+      <c r="B20" s="91"/>
+      <c r="C20" s="92"/>
+      <c r="D20" s="92">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="93"/>
+      <c r="F20" s="94"/>
+      <c r="G20" s="94"/>
+      <c r="H20" s="94"/>
+      <c r="I20" s="95"/>
     </row>
     <row r="21" spans="1:9" s="28" customFormat="1" ht="12.75">
       <c r="A21" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E21" s="35"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="37"/>
+      <c r="B21" s="91"/>
+      <c r="C21" s="92"/>
+      <c r="D21" s="92">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E21" s="93"/>
+      <c r="F21" s="94"/>
+      <c r="G21" s="94"/>
+      <c r="H21" s="94"/>
+      <c r="I21" s="95"/>
     </row>
     <row r="22" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A22" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E22" s="38"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="40"/>
+      <c r="B22" s="86"/>
+      <c r="C22" s="87"/>
+      <c r="D22" s="87">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="88"/>
+      <c r="F22" s="89"/>
+      <c r="G22" s="89"/>
+      <c r="H22" s="89"/>
+      <c r="I22" s="90"/>
     </row>
     <row r="23" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A23" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E23" s="38"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="40"/>
+      <c r="B23" s="86"/>
+      <c r="C23" s="87"/>
+      <c r="D23" s="87">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E23" s="88"/>
+      <c r="F23" s="89"/>
+      <c r="G23" s="89"/>
+      <c r="H23" s="89"/>
+      <c r="I23" s="90"/>
     </row>
     <row r="24" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A24" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="30">
+      <c r="B24" s="86">
         <v>0.54166666666666663</v>
       </c>
-      <c r="C24" s="31">
-        <v>0.625</v>
-      </c>
-      <c r="D24" s="31">
-        <f t="shared" si="0"/>
-        <v>8.333333333333337E-2</v>
-      </c>
-      <c r="E24" s="38" t="s">
+      <c r="C24" s="87">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D24" s="87">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+      <c r="E24" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="40"/>
+      <c r="F24" s="89"/>
+      <c r="G24" s="89"/>
+      <c r="H24" s="89"/>
+      <c r="I24" s="90"/>
     </row>
     <row r="25" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A25" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="30"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E25" s="38"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="40"/>
+      <c r="B25" s="86"/>
+      <c r="C25" s="87"/>
+      <c r="D25" s="87">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="88"/>
+      <c r="F25" s="89"/>
+      <c r="G25" s="89"/>
+      <c r="H25" s="89"/>
+      <c r="I25" s="90"/>
     </row>
     <row r="26" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A26" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E26" s="38"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="40"/>
+      <c r="B26" s="86"/>
+      <c r="C26" s="87"/>
+      <c r="D26" s="87">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E26" s="88"/>
+      <c r="F26" s="89"/>
+      <c r="G26" s="89"/>
+      <c r="H26" s="89"/>
+      <c r="I26" s="90"/>
     </row>
     <row r="27" spans="1:9" s="28" customFormat="1" ht="12.75">
       <c r="A27" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E27" s="35"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="37"/>
+      <c r="B27" s="91"/>
+      <c r="C27" s="92"/>
+      <c r="D27" s="92">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="93"/>
+      <c r="F27" s="94"/>
+      <c r="G27" s="94"/>
+      <c r="H27" s="94"/>
+      <c r="I27" s="95"/>
     </row>
     <row r="28" spans="1:9" s="28" customFormat="1" ht="12.75">
       <c r="A28" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E28" s="35"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="37"/>
+      <c r="B28" s="91"/>
+      <c r="C28" s="92"/>
+      <c r="D28" s="92">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E28" s="93"/>
+      <c r="F28" s="94"/>
+      <c r="G28" s="94"/>
+      <c r="H28" s="94"/>
+      <c r="I28" s="95"/>
     </row>
     <row r="29" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A29" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E29" s="38"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="40"/>
+      <c r="B29" s="86"/>
+      <c r="C29" s="87"/>
+      <c r="D29" s="87">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E29" s="88"/>
+      <c r="F29" s="89"/>
+      <c r="G29" s="89"/>
+      <c r="H29" s="89"/>
+      <c r="I29" s="90"/>
     </row>
     <row r="30" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A30" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="30">
+      <c r="B30" s="86">
         <v>0.54166666666666663</v>
       </c>
-      <c r="C30" s="31">
+      <c r="C30" s="87">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D30" s="31">
+      <c r="D30" s="87">
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
-      <c r="E30" s="38" t="s">
+      <c r="E30" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="40"/>
+      <c r="F30" s="89"/>
+      <c r="G30" s="89"/>
+      <c r="H30" s="89"/>
+      <c r="I30" s="90"/>
     </row>
     <row r="31" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A31" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E31" s="38"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="40"/>
+      <c r="B31" s="86"/>
+      <c r="C31" s="87"/>
+      <c r="D31" s="87">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E31" s="88"/>
+      <c r="F31" s="89"/>
+      <c r="G31" s="89"/>
+      <c r="H31" s="89"/>
+      <c r="I31" s="90"/>
     </row>
     <row r="32" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A32" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="30"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E32" s="38"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="40"/>
+      <c r="B32" s="86"/>
+      <c r="C32" s="87"/>
+      <c r="D32" s="87">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E32" s="88"/>
+      <c r="F32" s="89"/>
+      <c r="G32" s="89"/>
+      <c r="H32" s="89"/>
+      <c r="I32" s="90"/>
     </row>
     <row r="33" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A33" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="30"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E33" s="38"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="40"/>
+      <c r="B33" s="86"/>
+      <c r="C33" s="87"/>
+      <c r="D33" s="87">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E33" s="88"/>
+      <c r="F33" s="89"/>
+      <c r="G33" s="89"/>
+      <c r="H33" s="89"/>
+      <c r="I33" s="90"/>
     </row>
     <row r="34" spans="1:12" s="28" customFormat="1" ht="12.75">
       <c r="A34" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="26">
+      <c r="B34" s="91">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C34" s="27">
+      <c r="C34" s="92">
         <v>0.70833333333333337</v>
       </c>
-      <c r="D34" s="27">
+      <c r="D34" s="92">
         <f t="shared" si="0"/>
         <v>4.1666666666666741E-2</v>
       </c>
-      <c r="E34" s="35" t="s">
+      <c r="E34" s="93" t="s">
         <v>70</v>
       </c>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="37"/>
+      <c r="F34" s="94"/>
+      <c r="G34" s="94"/>
+      <c r="H34" s="94"/>
+      <c r="I34" s="95"/>
     </row>
     <row r="35" spans="1:12" s="28" customFormat="1" ht="12.75">
       <c r="A35" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="26"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E35" s="35"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="37"/>
+      <c r="B35" s="91"/>
+      <c r="C35" s="92"/>
+      <c r="D35" s="92">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E35" s="93"/>
+      <c r="F35" s="94"/>
+      <c r="G35" s="94"/>
+      <c r="H35" s="94"/>
+      <c r="I35" s="95"/>
     </row>
     <row r="36" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A36" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="30"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E36" s="38"/>
-      <c r="F36" s="39"/>
-      <c r="G36" s="39"/>
-      <c r="H36" s="39"/>
-      <c r="I36" s="40"/>
+      <c r="B36" s="86">
+        <v>0.5</v>
+      </c>
+      <c r="C36" s="87">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D36" s="87">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666663</v>
+      </c>
+      <c r="E36" s="88" t="s">
+        <v>71</v>
+      </c>
+      <c r="F36" s="89"/>
+      <c r="G36" s="89"/>
+      <c r="H36" s="89"/>
+      <c r="I36" s="90"/>
     </row>
     <row r="37" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A37" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="30"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E37" s="38"/>
-      <c r="F37" s="39"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="39"/>
-      <c r="I37" s="40"/>
+      <c r="B37" s="86">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C37" s="87">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D37" s="87">
+        <f t="shared" si="0"/>
+        <v>0.12499999999999994</v>
+      </c>
+      <c r="E37" s="88" t="s">
+        <v>72</v>
+      </c>
+      <c r="F37" s="89"/>
+      <c r="G37" s="89"/>
+      <c r="H37" s="89"/>
+      <c r="I37" s="90"/>
     </row>
     <row r="38" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A38" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="30"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E38" s="38"/>
-      <c r="F38" s="39"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="39"/>
-      <c r="I38" s="40"/>
+      <c r="B38" s="86">
+        <v>0.5</v>
+      </c>
+      <c r="C38" s="87">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D38" s="87">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E38" s="88" t="s">
+        <v>72</v>
+      </c>
+      <c r="F38" s="89"/>
+      <c r="G38" s="89"/>
+      <c r="H38" s="89"/>
+      <c r="I38" s="90"/>
     </row>
     <row r="39" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A39" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="30"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E39" s="38"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="39"/>
-      <c r="I39" s="40"/>
+      <c r="B39" s="86"/>
+      <c r="C39" s="87"/>
+      <c r="D39" s="87">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E39" s="88"/>
+      <c r="F39" s="89"/>
+      <c r="G39" s="89"/>
+      <c r="H39" s="89"/>
+      <c r="I39" s="90"/>
     </row>
     <row r="40" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A40" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B40" s="30"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E40" s="38"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="39"/>
-      <c r="H40" s="39"/>
-      <c r="I40" s="40"/>
+      <c r="B40" s="86"/>
+      <c r="C40" s="87"/>
+      <c r="D40" s="87">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E40" s="88"/>
+      <c r="F40" s="89"/>
+      <c r="G40" s="89"/>
+      <c r="H40" s="89"/>
+      <c r="I40" s="90"/>
     </row>
     <row r="41" spans="1:12" s="28" customFormat="1" ht="12.75">
       <c r="A41" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="26"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E41" s="35"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="37"/>
+      <c r="B41" s="91"/>
+      <c r="C41" s="92"/>
+      <c r="D41" s="92">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E41" s="93"/>
+      <c r="F41" s="94"/>
+      <c r="G41" s="94"/>
+      <c r="H41" s="94"/>
+      <c r="I41" s="95"/>
     </row>
     <row r="42" spans="1:12" s="28" customFormat="1" ht="12.75">
       <c r="A42" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="26"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E42" s="35"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="37"/>
+      <c r="B42" s="91"/>
+      <c r="C42" s="92"/>
+      <c r="D42" s="92">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E42" s="93"/>
+      <c r="F42" s="94"/>
+      <c r="G42" s="94"/>
+      <c r="H42" s="94"/>
+      <c r="I42" s="95"/>
     </row>
     <row r="43" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A43" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B43" s="30"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E43" s="38"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="39"/>
-      <c r="H43" s="39"/>
-      <c r="I43" s="40"/>
+      <c r="B43" s="86"/>
+      <c r="C43" s="87"/>
+      <c r="D43" s="87">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E43" s="88"/>
+      <c r="F43" s="89"/>
+      <c r="G43" s="89"/>
+      <c r="H43" s="89"/>
+      <c r="I43" s="90"/>
     </row>
     <row r="44" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A44" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="B44" s="30"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E44" s="38"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="40"/>
+      <c r="B44" s="86">
+        <v>0.5</v>
+      </c>
+      <c r="C44" s="87">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D44" s="87">
+        <f t="shared" si="0"/>
+        <v>0.10416666666666663</v>
+      </c>
+      <c r="E44" s="88" t="s">
+        <v>73</v>
+      </c>
+      <c r="F44" s="89"/>
+      <c r="G44" s="89"/>
+      <c r="H44" s="89"/>
+      <c r="I44" s="90"/>
     </row>
     <row r="45" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A45" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="30"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E45" s="38"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="39"/>
-      <c r="I45" s="40"/>
+      <c r="B45" s="86"/>
+      <c r="C45" s="87"/>
+      <c r="D45" s="87">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E45" s="88"/>
+      <c r="F45" s="89"/>
+      <c r="G45" s="89"/>
+      <c r="H45" s="89"/>
+      <c r="I45" s="90"/>
     </row>
     <row r="46" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A46" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B46" s="30"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E46" s="38"/>
-      <c r="F46" s="39"/>
-      <c r="G46" s="39"/>
-      <c r="H46" s="39"/>
-      <c r="I46" s="40"/>
+      <c r="B46" s="86"/>
+      <c r="C46" s="87"/>
+      <c r="D46" s="87">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E46" s="88"/>
+      <c r="F46" s="89"/>
+      <c r="G46" s="89"/>
+      <c r="H46" s="89"/>
+      <c r="I46" s="90"/>
     </row>
     <row r="47" spans="1:12" s="24" customFormat="1" ht="15">
-      <c r="A47" s="41"/>
-      <c r="B47" s="42"/>
-      <c r="C47" s="42"/>
+      <c r="A47" s="83"/>
+      <c r="B47" s="84"/>
+      <c r="C47" s="84"/>
       <c r="D47" s="23">
         <f>SUM(D16:D46)</f>
-        <v>0.4166666666666668</v>
-      </c>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="43"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="87"/>
+        <v>0.9375</v>
+      </c>
+      <c r="E47" s="85"/>
+      <c r="F47" s="85"/>
+      <c r="G47" s="85"/>
+      <c r="H47" s="85"/>
+      <c r="I47" s="97"/>
     </row>
     <row r="48" spans="1:12" ht="7.15" customHeight="1">
       <c r="A48" s="18"/>
@@ -3989,48 +4044,6 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E29:I29"/>
-    <mergeCell ref="E30:I30"/>
-    <mergeCell ref="E31:I31"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E35:I35"/>
-    <mergeCell ref="E36:I36"/>
-    <mergeCell ref="E37:I37"/>
-    <mergeCell ref="E32:I32"/>
-    <mergeCell ref="E33:I33"/>
-    <mergeCell ref="E34:I34"/>
-    <mergeCell ref="E41:I41"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="E38:I38"/>
-    <mergeCell ref="E39:I39"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="E47:I47"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="E45:I45"/>
-    <mergeCell ref="E46:I46"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:H7"/>
     <mergeCell ref="A8:I8"/>
@@ -4040,6 +4053,48 @@
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:I15"/>
     <mergeCell ref="A9:C9"/>
+    <mergeCell ref="E47:I47"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="E45:I45"/>
+    <mergeCell ref="E46:I46"/>
+    <mergeCell ref="E41:I41"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="E39:I39"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="E35:I35"/>
+    <mergeCell ref="E36:I36"/>
+    <mergeCell ref="E37:I37"/>
+    <mergeCell ref="E32:I32"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="E34:I34"/>
+    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="E31:I31"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:H5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.44" right="0.03" top="0.02" bottom="0.03" header="0.19685039370078741" footer="0.19685039370078741"/>
@@ -4074,18 +4129,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" s="6" customFormat="1" ht="18.75" thickBot="1">
-      <c r="A1" s="81" t="str">
+      <c r="A1" s="35" t="str">
         <f>October!A1</f>
         <v>Monthly timesheet for MSc Geoinformatics ip:sdi - 23W856162</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -4118,126 +4173,126 @@
       <c r="AM1" s="1"/>
     </row>
     <row r="2" spans="1:39" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A2" s="82"/>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
     </row>
     <row r="3" spans="1:39" s="7" customFormat="1" ht="13.7" customHeight="1">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="83"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="14"/>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
     </row>
     <row r="4" spans="1:39" s="1" customFormat="1" ht="9" customHeight="1">
-      <c r="A4" s="84"/>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
     </row>
     <row r="5" spans="1:39" s="1" customFormat="1" ht="13.9" customHeight="1">
-      <c r="A5" s="73" t="str">
+      <c r="A5" s="41" t="str">
         <f>October!A5</f>
         <v>Firstname Lastname</v>
       </c>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="75" t="str">
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="43" t="str">
         <f>October!D5</f>
         <v>Noah Greupner</v>
       </c>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="76"/>
-      <c r="H5" s="77"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="45"/>
       <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:39" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A6" s="78"/>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
     </row>
     <row r="7" spans="1:39" s="1" customFormat="1" ht="13.9" customHeight="1">
-      <c r="A7" s="79" t="str">
+      <c r="A7" s="47" t="str">
         <f>October!A7</f>
         <v>Project Acronym</v>
       </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="80" t="str">
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="48" t="str">
         <f>October!D7</f>
         <v>SudMig</v>
       </c>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="80"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
       <c r="I7" s="15"/>
     </row>
     <row r="8" spans="1:39" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A8" s="85"/>
-      <c r="B8" s="85"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="85"/>
-      <c r="H8" s="85"/>
-      <c r="I8" s="85"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
     </row>
     <row r="9" spans="1:39" s="1" customFormat="1" ht="13.9" customHeight="1">
-      <c r="A9" s="79" t="str">
+      <c r="A9" s="47" t="str">
         <f>October!A9</f>
         <v>Project Title</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="75" t="str">
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="43" t="str">
         <f>October!D9</f>
         <v>Sudan: monitoring migrant movements related to the 2023 conflict</v>
       </c>
-      <c r="E9" s="76"/>
-      <c r="F9" s="76"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="77"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="45"/>
       <c r="I9" s="15"/>
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:39" s="1" customFormat="1" ht="7.5" customHeight="1">
-      <c r="A10" s="72"/>
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="72"/>
-      <c r="G10" s="72"/>
-      <c r="H10" s="72"/>
-      <c r="I10" s="72"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
     </row>
     <row r="11" spans="1:39" s="1" customFormat="1" ht="12.75">
       <c r="A11" s="34" t="s">
@@ -4267,51 +4322,51 @@
       <c r="I12" s="16"/>
     </row>
     <row r="13" spans="1:39" s="2" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="60" t="s">
+      <c r="B13" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="62"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="54"/>
     </row>
     <row r="14" spans="1:39" s="2" customFormat="1" ht="13.9" customHeight="1">
-      <c r="A14" s="58"/>
-      <c r="B14" s="63" t="s">
+      <c r="A14" s="50"/>
+      <c r="B14" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="86"/>
-      <c r="D14" s="64" t="s">
+      <c r="C14" s="96"/>
+      <c r="D14" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="66" t="s">
+      <c r="E14" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="67"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="67"/>
-      <c r="I14" s="68"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="60"/>
     </row>
     <row r="15" spans="1:39" ht="13.35" customHeight="1">
-      <c r="A15" s="59"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="65"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="70"/>
-      <c r="H15" s="70"/>
-      <c r="I15" s="71"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="63"/>
     </row>
     <row r="16" spans="1:39" s="32" customFormat="1" ht="12.75">
       <c r="A16" s="29" t="s">
@@ -4323,11 +4378,11 @@
         <f>C16-B16</f>
         <v>0</v>
       </c>
-      <c r="E16" s="38"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="40"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="71"/>
+      <c r="G16" s="71"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="72"/>
     </row>
     <row r="17" spans="1:9" s="28" customFormat="1" ht="12.75">
       <c r="A17" s="25" t="s">
@@ -4339,11 +4394,11 @@
         <f t="shared" ref="D17:D45" si="0">C17-B17</f>
         <v>0</v>
       </c>
-      <c r="E17" s="35"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="37"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="69"/>
     </row>
     <row r="18" spans="1:9" s="28" customFormat="1" ht="12.75">
       <c r="A18" s="25" t="s">
@@ -4355,11 +4410,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E18" s="35"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="37"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="69"/>
     </row>
     <row r="19" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A19" s="29" t="s">
@@ -4371,11 +4426,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E19" s="38"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="40"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="72"/>
     </row>
     <row r="20" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A20" s="29" t="s">
@@ -4387,11 +4442,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="40"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="72"/>
     </row>
     <row r="21" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A21" s="29" t="s">
@@ -4403,11 +4458,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E21" s="38"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="40"/>
+      <c r="E21" s="70"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="72"/>
     </row>
     <row r="22" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A22" s="29" t="s">
@@ -4419,11 +4474,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E22" s="38"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="40"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="72"/>
     </row>
     <row r="23" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A23" s="29" t="s">
@@ -4435,11 +4490,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E23" s="38"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="40"/>
+      <c r="E23" s="70"/>
+      <c r="F23" s="71"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="72"/>
     </row>
     <row r="24" spans="1:9" s="28" customFormat="1" ht="12.75">
       <c r="A24" s="25" t="s">
@@ -4451,11 +4506,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E24" s="35"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="37"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="69"/>
     </row>
     <row r="25" spans="1:9" s="28" customFormat="1" ht="12.75">
       <c r="A25" s="25" t="s">
@@ -4467,11 +4522,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E25" s="35"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="37"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="69"/>
     </row>
     <row r="26" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A26" s="29" t="s">
@@ -4483,11 +4538,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E26" s="38"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="40"/>
+      <c r="E26" s="70"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="72"/>
     </row>
     <row r="27" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A27" s="29" t="s">
@@ -4499,11 +4554,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27" s="38"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="40"/>
+      <c r="E27" s="70"/>
+      <c r="F27" s="71"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="71"/>
+      <c r="I27" s="72"/>
     </row>
     <row r="28" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A28" s="29" t="s">
@@ -4515,11 +4570,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E28" s="38"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="40"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="72"/>
     </row>
     <row r="29" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A29" s="29" t="s">
@@ -4531,11 +4586,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E29" s="38"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="40"/>
+      <c r="E29" s="70"/>
+      <c r="F29" s="71"/>
+      <c r="G29" s="71"/>
+      <c r="H29" s="71"/>
+      <c r="I29" s="72"/>
     </row>
     <row r="30" spans="1:9" s="32" customFormat="1" ht="12.75">
       <c r="A30" s="29" t="s">
@@ -4547,11 +4602,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E30" s="38"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="40"/>
+      <c r="E30" s="70"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="72"/>
     </row>
     <row r="31" spans="1:9" s="28" customFormat="1" ht="12.75">
       <c r="A31" s="25" t="s">
@@ -4563,11 +4618,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E31" s="35"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="37"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="68"/>
+      <c r="G31" s="68"/>
+      <c r="H31" s="68"/>
+      <c r="I31" s="69"/>
     </row>
     <row r="32" spans="1:9" s="28" customFormat="1" ht="12.75">
       <c r="A32" s="25" t="s">
@@ -4579,11 +4634,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E32" s="35"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="37"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="68"/>
+      <c r="G32" s="68"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="69"/>
     </row>
     <row r="33" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A33" s="29" t="s">
@@ -4595,11 +4650,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E33" s="38"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="40"/>
+      <c r="E33" s="70"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="71"/>
+      <c r="I33" s="72"/>
     </row>
     <row r="34" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A34" s="29" t="s">
@@ -4611,11 +4666,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E34" s="38"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="39"/>
-      <c r="I34" s="40"/>
+      <c r="E34" s="70"/>
+      <c r="F34" s="71"/>
+      <c r="G34" s="71"/>
+      <c r="H34" s="71"/>
+      <c r="I34" s="72"/>
     </row>
     <row r="35" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A35" s="29" t="s">
@@ -4627,11 +4682,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E35" s="38"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="40"/>
+      <c r="E35" s="70"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="71"/>
+      <c r="H35" s="71"/>
+      <c r="I35" s="72"/>
     </row>
     <row r="36" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A36" s="29" t="s">
@@ -4643,11 +4698,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E36" s="38"/>
-      <c r="F36" s="39"/>
-      <c r="G36" s="39"/>
-      <c r="H36" s="39"/>
-      <c r="I36" s="40"/>
+      <c r="E36" s="70"/>
+      <c r="F36" s="71"/>
+      <c r="G36" s="71"/>
+      <c r="H36" s="71"/>
+      <c r="I36" s="72"/>
     </row>
     <row r="37" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A37" s="29" t="s">
@@ -4659,11 +4714,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E37" s="38"/>
-      <c r="F37" s="39"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="39"/>
-      <c r="I37" s="40"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="71"/>
+      <c r="G37" s="71"/>
+      <c r="H37" s="71"/>
+      <c r="I37" s="72"/>
     </row>
     <row r="38" spans="1:12" s="28" customFormat="1" ht="12.75">
       <c r="A38" s="25" t="s">
@@ -4675,11 +4730,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E38" s="35"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="37"/>
+      <c r="E38" s="67"/>
+      <c r="F38" s="68"/>
+      <c r="G38" s="68"/>
+      <c r="H38" s="68"/>
+      <c r="I38" s="69"/>
     </row>
     <row r="39" spans="1:12" s="28" customFormat="1" ht="12.75">
       <c r="A39" s="25" t="s">
@@ -4691,11 +4746,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E39" s="35"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="37"/>
+      <c r="E39" s="67"/>
+      <c r="F39" s="68"/>
+      <c r="G39" s="68"/>
+      <c r="H39" s="68"/>
+      <c r="I39" s="69"/>
     </row>
     <row r="40" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A40" s="29" t="s">
@@ -4707,11 +4762,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E40" s="38"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="39"/>
-      <c r="H40" s="39"/>
-      <c r="I40" s="40"/>
+      <c r="E40" s="70"/>
+      <c r="F40" s="71"/>
+      <c r="G40" s="71"/>
+      <c r="H40" s="71"/>
+      <c r="I40" s="72"/>
     </row>
     <row r="41" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A41" s="29" t="s">
@@ -4723,11 +4778,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E41" s="38"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="39"/>
-      <c r="H41" s="39"/>
-      <c r="I41" s="40"/>
+      <c r="E41" s="70"/>
+      <c r="F41" s="71"/>
+      <c r="G41" s="71"/>
+      <c r="H41" s="71"/>
+      <c r="I41" s="72"/>
     </row>
     <row r="42" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A42" s="29" t="s">
@@ -4739,11 +4794,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E42" s="38"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="39"/>
-      <c r="I42" s="40"/>
+      <c r="E42" s="70"/>
+      <c r="F42" s="71"/>
+      <c r="G42" s="71"/>
+      <c r="H42" s="71"/>
+      <c r="I42" s="72"/>
     </row>
     <row r="43" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A43" s="29" t="s">
@@ -4755,11 +4810,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E43" s="38"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="39"/>
-      <c r="H43" s="39"/>
-      <c r="I43" s="40"/>
+      <c r="E43" s="70"/>
+      <c r="F43" s="71"/>
+      <c r="G43" s="71"/>
+      <c r="H43" s="71"/>
+      <c r="I43" s="72"/>
     </row>
     <row r="44" spans="1:12" s="32" customFormat="1" ht="12.75">
       <c r="A44" s="29" t="s">
@@ -4771,11 +4826,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E44" s="38"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="40"/>
+      <c r="E44" s="70"/>
+      <c r="F44" s="71"/>
+      <c r="G44" s="71"/>
+      <c r="H44" s="71"/>
+      <c r="I44" s="72"/>
     </row>
     <row r="45" spans="1:12" s="28" customFormat="1" ht="12.75">
       <c r="A45" s="25" t="s">
@@ -4787,25 +4842,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E45" s="35"/>
-      <c r="F45" s="36"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="37"/>
+      <c r="E45" s="67"/>
+      <c r="F45" s="68"/>
+      <c r="G45" s="68"/>
+      <c r="H45" s="68"/>
+      <c r="I45" s="69"/>
     </row>
     <row r="46" spans="1:12" s="24" customFormat="1" ht="15">
-      <c r="A46" s="41"/>
-      <c r="B46" s="42"/>
-      <c r="C46" s="42"/>
+      <c r="A46" s="83"/>
+      <c r="B46" s="84"/>
+      <c r="C46" s="84"/>
       <c r="D46" s="23">
         <f>SUM(D16:D45)</f>
         <v>0</v>
       </c>
-      <c r="E46" s="43"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="43"/>
-      <c r="H46" s="43"/>
-      <c r="I46" s="87"/>
+      <c r="E46" s="85"/>
+      <c r="F46" s="85"/>
+      <c r="G46" s="85"/>
+      <c r="H46" s="85"/>
+      <c r="I46" s="97"/>
     </row>
     <row r="47" spans="1:12" ht="7.15" customHeight="1">
       <c r="A47" s="18"/>
@@ -4823,24 +4878,26 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:I15"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="E46:I46"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="E41:I41"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="E45:I45"/>
+    <mergeCell ref="E39:I39"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="E31:I31"/>
+    <mergeCell ref="E32:I32"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="E34:I34"/>
+    <mergeCell ref="E35:I35"/>
+    <mergeCell ref="E36:I36"/>
+    <mergeCell ref="E37:I37"/>
+    <mergeCell ref="E38:I38"/>
     <mergeCell ref="E27:I27"/>
     <mergeCell ref="E16:I16"/>
     <mergeCell ref="E17:I17"/>
@@ -4853,26 +4910,24 @@
     <mergeCell ref="E24:I24"/>
     <mergeCell ref="E25:I25"/>
     <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E39:I39"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
-    <mergeCell ref="E30:I30"/>
-    <mergeCell ref="E31:I31"/>
-    <mergeCell ref="E32:I32"/>
-    <mergeCell ref="E33:I33"/>
-    <mergeCell ref="E34:I34"/>
-    <mergeCell ref="E35:I35"/>
-    <mergeCell ref="E36:I36"/>
-    <mergeCell ref="E37:I37"/>
-    <mergeCell ref="E38:I38"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="E46:I46"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="E41:I41"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="E45:I45"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:I15"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:H5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.44" right="0.03" top="0.02" bottom="0.03" header="0.19685039370078741" footer="0.19685039370078741"/>
@@ -4882,26 +4937,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="34840fcf-b2b1-4e6c-965a-1d79bbd7ca53">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="efe5fd09-895f-413c-ad62-8a7b7313e3f2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E194172A664C3D44B55AD259CF5259CC" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a3a3b985f66752244a6c0b9bb1957eb4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="efe5fd09-895f-413c-ad62-8a7b7313e3f2" xmlns:ns3="34840fcf-b2b1-4e6c-965a-1d79bbd7ca53" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1f1f5da211ee33ec20a81d51d442b62d" ns2:_="" ns3:_="">
     <xsd:import namespace="efe5fd09-895f-413c-ad62-8a7b7313e3f2"/>
@@ -5112,8 +5147,28 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="34840fcf-b2b1-4e6c-965a-1d79bbd7ca53">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="efe5fd09-895f-413c-ad62-8a7b7313e3f2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5C6E515-50F4-4AD4-95A5-0F833900AC83}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F961F73-87F5-4681-8DB3-9613597406C2}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5121,5 +5176,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F961F73-87F5-4681-8DB3-9613597406C2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5C6E515-50F4-4AD4-95A5-0F833900AC83}"/>
 </file>
</xml_diff>